<commit_message>
Refactor pastry data into shared property PastryData
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Other/PivotTableReferenceFiles/SourceSheetWithWhitespace/outputfile.xlsx
+++ b/ClosedXML_Tests/Resource/Other/PivotTableReferenceFiles/SourceSheetWithWhitespace/outputfile.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -39,6 +39,15 @@
   </x:si>
   <x:si>
     <x:t>Croissant</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Apr</x:t>
+  </x:si>
+  <x:si>
+    <x:t>May</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jun</x:t>
   </x:si>
   <x:si>
     <x:t>Doughnut</x:t>
@@ -120,7 +129,7 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -147,14 +156,28 @@
     <x:pivotField name="Code" defaultSubtotal="0"/>
     <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
     <x:pivotField name="Quality" defaultSubtotal="0"/>
-    <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0"/>
+    <x:pivotField name="Month" axis="axisRow" showAll="0" defaultSubtotal="0">
+      <x:items count="3">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+      </x:items>
+    </x:pivotField>
     <x:pivotField name="BakeDate" defaultSubtotal="0"/>
   </x:pivotFields>
   <x:rowFields count="1">
     <x:field x="4"/>
   </x:rowFields>
-  <x:rowItems count="2">
-    <x:i/>
+  <x:rowItems count="4">
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
     <x:i t="grand">
       <x:x/>
     </x:i>
@@ -544,6 +567,9 @@
       <x:c r="D2" s="0" t="n">
         <x:v>60.2</x:v>
       </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
       <x:c r="F2" s="1">
         <x:v>42481</x:v>
       </x:c>
@@ -561,6 +587,9 @@
       <x:c r="D3" s="0" t="n">
         <x:v>50.42</x:v>
       </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
       <x:c r="F3" s="1">
         <x:v>42493</x:v>
       </x:c>
@@ -578,13 +607,16 @@
       <x:c r="D4" s="0" t="n">
         <x:v>22.12</x:v>
       </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
       <x:c r="F4" s="1">
         <x:v>42545</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6">
       <x:c r="A5" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B5" s="0" t="n">
         <x:v>102</x:v>
@@ -595,13 +627,16 @@
       <x:c r="D5" s="0" t="n">
         <x:v>89.99</x:v>
       </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
       <x:c r="F5" s="1">
         <x:v>42848</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6">
       <x:c r="A6" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B6" s="0" t="n">
         <x:v>102</x:v>
@@ -612,13 +647,16 @@
       <x:c r="D6" s="0" t="n">
         <x:v>70</x:v>
       </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
       <x:c r="F6" s="1">
         <x:v>42514</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6">
       <x:c r="A7" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B7" s="0" t="n">
         <x:v>102</x:v>
@@ -629,13 +667,16 @@
       <x:c r="D7" s="0" t="n">
         <x:v>75.33</x:v>
       </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
       <x:c r="F7" s="1">
         <x:v>42523</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:6">
       <x:c r="A8" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B8" s="0" t="n">
         <x:v>103</x:v>
@@ -646,13 +687,16 @@
       <x:c r="D8" s="0" t="n">
         <x:v>10.24</x:v>
       </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
       <x:c r="F8" s="1">
         <x:v>42487</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:6">
       <x:c r="A9" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B9" s="0" t="n">
         <x:v>103</x:v>
@@ -663,13 +707,16 @@
       <x:c r="D9" s="0" t="n">
         <x:v>33.33</x:v>
       </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
       <x:c r="F9" s="1">
         <x:v>42510</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:6">
       <x:c r="A10" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B10" s="0" t="n">
         <x:v>103</x:v>
@@ -680,13 +727,16 @@
       <x:c r="D10" s="0" t="n">
         <x:v>25</x:v>
       </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
       <x:c r="F10" s="1">
         <x:v>42891</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:6">
       <x:c r="A11" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B11" s="0" t="n">
         <x:v>104</x:v>
@@ -697,11 +747,16 @@
       <x:c r="D11" s="0" t="n">
         <x:v>-20.24</x:v>
       </x:c>
-      <x:c r="F11" s="2" t="s"/>
+      <x:c r="E11" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="F11" s="2">
+        <x:v>42849</x:v>
+      </x:c>
     </x:row>
     <x:row r="12" spans="1:6">
       <x:c r="A12" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B12" s="0" t="n">
         <x:v>104</x:v>
@@ -712,13 +767,16 @@
       <x:c r="D12" s="0" t="n">
         <x:v>60</x:v>
       </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
       <x:c r="F12" s="1">
         <x:v>42863</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:6">
       <x:c r="A13" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="0" t="n">
         <x:v>104</x:v>
@@ -729,13 +787,16 @@
       <x:c r="D13" s="0" t="n">
         <x:v>24.76</x:v>
       </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
       <x:c r="F13" s="1">
         <x:v>42542</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:6">
       <x:c r="A14" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B14" s="0" t="n">
         <x:v>105</x:v>
@@ -746,13 +807,16 @@
       <x:c r="D14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
       <x:c r="F14" s="1">
         <x:v>42847</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:6">
       <x:c r="A15" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B15" s="0" t="n">
         <x:v>105</x:v>
@@ -763,13 +827,16 @@
       <x:c r="D15" s="0" t="n">
         <x:v>5.19</x:v>
       </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
       <x:c r="F15" s="1">
         <x:v>42858</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:6">
       <x:c r="A16" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B16" s="0" t="n">
         <x:v>105</x:v>
@@ -780,13 +847,16 @@
       <x:c r="D16" s="0" t="n">
         <x:v>44.2</x:v>
       </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
       <x:c r="F16" s="1">
         <x:v>42900</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:6">
       <x:c r="A17" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C17" s="0" t="n">
         <x:v>255</x:v>
@@ -853,10 +923,14 @@
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
     </x:cacheField>
     <x:cacheField name="Month">
-      <x:sharedItems containsBlank="1"/>
+      <x:sharedItems count="3">
+        <x:s v="Apr"/>
+        <x:s v="May"/>
+        <x:s v="Jun"/>
+      </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="14"/>
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>

</xml_diff>